<commit_message>
Se agrega carousel de videos
</commit_message>
<xml_diff>
--- a/Entregables/Sprint 0/Historias de usuario.xlsx
+++ b/Entregables/Sprint 0/Historias de usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\Cursos\Mision Tic 2022\Ciclo 4\Proyecto\Entregables\Sprint 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F0F23B-F944-4756-8B58-A134C5E11CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D952A70C-B086-4005-8DE8-1717EF18E1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BDE8FFE-49EB-4574-A2FC-944E22EDA3E9}"/>
   </bookViews>
@@ -448,30 +448,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,6 +473,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,7 +933,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +944,7 @@
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="11" width="21" customWidth="1"/>
-    <col min="12" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1833,10 +1833,10 @@
       <c r="AA3" s="6"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="6">
         <v>1</v>
       </c>
@@ -1845,10 +1845,10 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="34"/>
       <c r="J4" s="6">
         <v>1</v>
       </c>
@@ -1857,10 +1857,10 @@
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="25"/>
+      <c r="P4" s="34"/>
       <c r="Q4" s="6">
         <v>1</v>
       </c>
@@ -1869,10 +1869,10 @@
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="W4" s="25"/>
+      <c r="W4" s="34"/>
       <c r="X4" s="6">
         <v>1</v>
       </c>
@@ -1975,272 +1975,272 @@
       <c r="AA6" s="11"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="28"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="28"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="20"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="20"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="31"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="31"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="23"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="23"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="23"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="31"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="31"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="31"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="23"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="23"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="31"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="31"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="23"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="23"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="23"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="31"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="31"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="31"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="23"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="23"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="23"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="31"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="31"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="23"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="23"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="23"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="23"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="31"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="31"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30"/>
-      <c r="AA13" s="31"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="23"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="23"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="34"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="34"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="33"/>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="34"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="26"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="26"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="26"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-      <c r="H15" s="18" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="H15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="O15" s="18" t="s">
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+      <c r="O15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="20"/>
-      <c r="V15" s="18" t="s">
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="29"/>
+      <c r="V15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="20"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="29"/>
     </row>
     <row r="16" spans="1:27" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="23"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="23"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="23"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="32"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="32"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2373,10 +2373,10 @@
       <c r="AA20" s="6"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="6">
         <v>1</v>
       </c>
@@ -2385,10 +2385,10 @@
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6"/>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="25"/>
+      <c r="I21" s="34"/>
       <c r="J21" s="6">
         <v>1</v>
       </c>
@@ -2397,10 +2397,10 @@
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="6"/>
-      <c r="O21" s="24" t="s">
+      <c r="O21" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="25"/>
+      <c r="P21" s="34"/>
       <c r="Q21" s="6">
         <v>1</v>
       </c>
@@ -2409,10 +2409,10 @@
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="6"/>
-      <c r="V21" s="24" t="s">
+      <c r="V21" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="W21" s="25"/>
+      <c r="W21" s="34"/>
       <c r="X21" s="6">
         <v>1</v>
       </c>
@@ -2515,272 +2515,272 @@
       <c r="AA23" s="11"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="28"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="28"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="20"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="20"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="20"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="31"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="31"/>
-      <c r="V25" s="29"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="31"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="23"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="23"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="22"/>
+      <c r="X25" s="22"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="23"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="31"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="31"/>
-      <c r="V26" s="29"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="31"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="23"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="23"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="23"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="31"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="31"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="31"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="23"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="23"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="23"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="31"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="31"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="31"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="23"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="23"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="23"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="31"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="31"/>
-      <c r="V29" s="29"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="31"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="23"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="23"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="23"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="31"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="31"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-      <c r="AA30" s="31"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="23"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="23"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="22"/>
+      <c r="X30" s="22"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="23"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="34"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
-      <c r="S31" s="33"/>
-      <c r="T31" s="34"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="33"/>
-      <c r="X31" s="33"/>
-      <c r="Y31" s="33"/>
-      <c r="Z31" s="33"/>
-      <c r="AA31" s="34"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="26"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="25"/>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AA31" s="26"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
-      <c r="H32" s="18" t="s">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29"/>
+      <c r="H32" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="20"/>
-      <c r="O32" s="18" t="s">
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="29"/>
+      <c r="O32" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="20"/>
-      <c r="V32" s="18" t="s">
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="29"/>
+      <c r="V32" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
-      <c r="AA32" s="20"/>
+      <c r="W32" s="28"/>
+      <c r="X32" s="28"/>
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="28"/>
+      <c r="AA32" s="29"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="23"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="23"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="22"/>
-      <c r="X33" s="22"/>
-      <c r="Y33" s="22"/>
-      <c r="Z33" s="22"/>
-      <c r="AA33" s="23"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="32"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="31"/>
+      <c r="Y33" s="31"/>
+      <c r="Z33" s="31"/>
+      <c r="AA33" s="32"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -2913,10 +2913,10 @@
       <c r="AA37" s="6"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="25"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="6">
         <v>1</v>
       </c>
@@ -2925,10 +2925,10 @@
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="6"/>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I38" s="25"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="6">
         <v>1</v>
       </c>
@@ -2937,10 +2937,10 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="6"/>
-      <c r="O38" s="24" t="s">
+      <c r="O38" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="P38" s="25"/>
+      <c r="P38" s="34"/>
       <c r="Q38" s="6">
         <v>1</v>
       </c>
@@ -2949,10 +2949,10 @@
       </c>
       <c r="S38" s="5"/>
       <c r="T38" s="6"/>
-      <c r="V38" s="24" t="s">
+      <c r="V38" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="W38" s="25"/>
+      <c r="W38" s="34"/>
       <c r="X38" s="6">
         <v>1</v>
       </c>
@@ -3055,272 +3055,272 @@
       <c r="AA40" s="11"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="28"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="28"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="28"/>
-      <c r="V41" s="26"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="28"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="20"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="20"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="19"/>
+      <c r="AA41" s="20"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="31"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="31"/>
-      <c r="O42" s="29"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="30"/>
-      <c r="S42" s="30"/>
-      <c r="T42" s="31"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="30"/>
-      <c r="X42" s="30"/>
-      <c r="Y42" s="30"/>
-      <c r="Z42" s="30"/>
-      <c r="AA42" s="31"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="23"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="23"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="23"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="22"/>
+      <c r="X42" s="22"/>
+      <c r="Y42" s="22"/>
+      <c r="Z42" s="22"/>
+      <c r="AA42" s="23"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="31"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="31"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="30"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="30"/>
-      <c r="Z43" s="30"/>
-      <c r="AA43" s="31"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="23"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="23"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="23"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
+      <c r="Z43" s="22"/>
+      <c r="AA43" s="23"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="31"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="31"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="30"/>
-      <c r="X44" s="30"/>
-      <c r="Y44" s="30"/>
-      <c r="Z44" s="30"/>
-      <c r="AA44" s="31"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="23"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="23"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="22"/>
+      <c r="Y44" s="22"/>
+      <c r="Z44" s="22"/>
+      <c r="AA44" s="23"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="31"/>
-      <c r="O45" s="29"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="30"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="31"/>
-      <c r="V45" s="29"/>
-      <c r="W45" s="30"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="30"/>
-      <c r="Z45" s="30"/>
-      <c r="AA45" s="31"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="23"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="23"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="23"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="22"/>
+      <c r="X45" s="22"/>
+      <c r="Y45" s="22"/>
+      <c r="Z45" s="22"/>
+      <c r="AA45" s="23"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="31"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="31"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="31"/>
-      <c r="V46" s="29"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="30"/>
-      <c r="Z46" s="30"/>
-      <c r="AA46" s="31"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="23"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="23"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="22"/>
+      <c r="Y46" s="22"/>
+      <c r="Z46" s="22"/>
+      <c r="AA46" s="23"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="31"/>
-      <c r="O47" s="29"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="30"/>
-      <c r="S47" s="30"/>
-      <c r="T47" s="31"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="30"/>
-      <c r="X47" s="30"/>
-      <c r="Y47" s="30"/>
-      <c r="Z47" s="30"/>
-      <c r="AA47" s="31"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="23"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="23"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="23"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="22"/>
+      <c r="X47" s="22"/>
+      <c r="Y47" s="22"/>
+      <c r="Z47" s="22"/>
+      <c r="AA47" s="23"/>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="34"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
-      <c r="R48" s="33"/>
-      <c r="S48" s="33"/>
-      <c r="T48" s="34"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="33"/>
-      <c r="X48" s="33"/>
-      <c r="Y48" s="33"/>
-      <c r="Z48" s="33"/>
-      <c r="AA48" s="34"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="26"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="26"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="25"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="25"/>
+      <c r="S48" s="25"/>
+      <c r="T48" s="26"/>
+      <c r="V48" s="24"/>
+      <c r="W48" s="25"/>
+      <c r="X48" s="25"/>
+      <c r="Y48" s="25"/>
+      <c r="Z48" s="25"/>
+      <c r="AA48" s="26"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="20"/>
-      <c r="H49" s="18" t="s">
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
+      <c r="H49" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="19"/>
-      <c r="M49" s="20"/>
-      <c r="O49" s="18" t="s">
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="29"/>
+      <c r="O49" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P49" s="19"/>
-      <c r="Q49" s="19"/>
-      <c r="R49" s="19"/>
-      <c r="S49" s="19"/>
-      <c r="T49" s="20"/>
-      <c r="V49" s="18" t="s">
+      <c r="P49" s="28"/>
+      <c r="Q49" s="28"/>
+      <c r="R49" s="28"/>
+      <c r="S49" s="28"/>
+      <c r="T49" s="29"/>
+      <c r="V49" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="W49" s="19"/>
-      <c r="X49" s="19"/>
-      <c r="Y49" s="19"/>
-      <c r="Z49" s="19"/>
-      <c r="AA49" s="20"/>
+      <c r="W49" s="28"/>
+      <c r="X49" s="28"/>
+      <c r="Y49" s="28"/>
+      <c r="Z49" s="28"/>
+      <c r="AA49" s="29"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="23"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="23"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-      <c r="T50" s="23"/>
-      <c r="V50" s="21"/>
-      <c r="W50" s="22"/>
-      <c r="X50" s="22"/>
-      <c r="Y50" s="22"/>
-      <c r="Z50" s="22"/>
-      <c r="AA50" s="23"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="32"/>
+      <c r="O50" s="30"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="31"/>
+      <c r="T50" s="32"/>
+      <c r="V50" s="30"/>
+      <c r="W50" s="31"/>
+      <c r="X50" s="31"/>
+      <c r="Y50" s="31"/>
+      <c r="Z50" s="31"/>
+      <c r="AA50" s="32"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -3453,10 +3453,10 @@
       <c r="AA54" s="6"/>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="34"/>
       <c r="C55" s="6">
         <v>1</v>
       </c>
@@ -3465,10 +3465,10 @@
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="6"/>
-      <c r="H55" s="24" t="s">
+      <c r="H55" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I55" s="25"/>
+      <c r="I55" s="34"/>
       <c r="J55" s="6">
         <v>1</v>
       </c>
@@ -3477,10 +3477,10 @@
       </c>
       <c r="L55" s="5"/>
       <c r="M55" s="6"/>
-      <c r="O55" s="24" t="s">
+      <c r="O55" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="P55" s="25"/>
+      <c r="P55" s="34"/>
       <c r="Q55" s="6">
         <v>1</v>
       </c>
@@ -3489,10 +3489,10 @@
       </c>
       <c r="S55" s="5"/>
       <c r="T55" s="6"/>
-      <c r="V55" s="24" t="s">
+      <c r="V55" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="W55" s="25"/>
+      <c r="W55" s="34"/>
       <c r="X55" s="6">
         <v>1</v>
       </c>
@@ -3595,311 +3595,275 @@
       <c r="AA57" s="11"/>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="28"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="28"/>
-      <c r="O58" s="26"/>
-      <c r="P58" s="27"/>
-      <c r="Q58" s="27"/>
-      <c r="R58" s="27"/>
-      <c r="S58" s="27"/>
-      <c r="T58" s="28"/>
-      <c r="V58" s="26"/>
-      <c r="W58" s="27"/>
-      <c r="X58" s="27"/>
-      <c r="Y58" s="27"/>
-      <c r="Z58" s="27"/>
-      <c r="AA58" s="28"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="20"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="20"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="19"/>
+      <c r="S58" s="19"/>
+      <c r="T58" s="20"/>
+      <c r="V58" s="18"/>
+      <c r="W58" s="19"/>
+      <c r="X58" s="19"/>
+      <c r="Y58" s="19"/>
+      <c r="Z58" s="19"/>
+      <c r="AA58" s="20"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="31"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="30"/>
-      <c r="M59" s="31"/>
-      <c r="O59" s="29"/>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="30"/>
-      <c r="R59" s="30"/>
-      <c r="S59" s="30"/>
-      <c r="T59" s="31"/>
-      <c r="V59" s="29"/>
-      <c r="W59" s="30"/>
-      <c r="X59" s="30"/>
-      <c r="Y59" s="30"/>
-      <c r="Z59" s="30"/>
-      <c r="AA59" s="31"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="23"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="23"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="22"/>
+      <c r="T59" s="23"/>
+      <c r="V59" s="21"/>
+      <c r="W59" s="22"/>
+      <c r="X59" s="22"/>
+      <c r="Y59" s="22"/>
+      <c r="Z59" s="22"/>
+      <c r="AA59" s="23"/>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="31"/>
-      <c r="O60" s="29"/>
-      <c r="P60" s="30"/>
-      <c r="Q60" s="30"/>
-      <c r="R60" s="30"/>
-      <c r="S60" s="30"/>
-      <c r="T60" s="31"/>
-      <c r="V60" s="29"/>
-      <c r="W60" s="30"/>
-      <c r="X60" s="30"/>
-      <c r="Y60" s="30"/>
-      <c r="Z60" s="30"/>
-      <c r="AA60" s="31"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="23"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="23"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
+      <c r="S60" s="22"/>
+      <c r="T60" s="23"/>
+      <c r="V60" s="21"/>
+      <c r="W60" s="22"/>
+      <c r="X60" s="22"/>
+      <c r="Y60" s="22"/>
+      <c r="Z60" s="22"/>
+      <c r="AA60" s="23"/>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="31"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-      <c r="L61" s="30"/>
-      <c r="M61" s="31"/>
-      <c r="O61" s="29"/>
-      <c r="P61" s="30"/>
-      <c r="Q61" s="30"/>
-      <c r="R61" s="30"/>
-      <c r="S61" s="30"/>
-      <c r="T61" s="31"/>
-      <c r="V61" s="29"/>
-      <c r="W61" s="30"/>
-      <c r="X61" s="30"/>
-      <c r="Y61" s="30"/>
-      <c r="Z61" s="30"/>
-      <c r="AA61" s="31"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="23"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="23"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+      <c r="S61" s="22"/>
+      <c r="T61" s="23"/>
+      <c r="V61" s="21"/>
+      <c r="W61" s="22"/>
+      <c r="X61" s="22"/>
+      <c r="Y61" s="22"/>
+      <c r="Z61" s="22"/>
+      <c r="AA61" s="23"/>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="31"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
-      <c r="L62" s="30"/>
-      <c r="M62" s="31"/>
-      <c r="O62" s="29"/>
-      <c r="P62" s="30"/>
-      <c r="Q62" s="30"/>
-      <c r="R62" s="30"/>
-      <c r="S62" s="30"/>
-      <c r="T62" s="31"/>
-      <c r="V62" s="29"/>
-      <c r="W62" s="30"/>
-      <c r="X62" s="30"/>
-      <c r="Y62" s="30"/>
-      <c r="Z62" s="30"/>
-      <c r="AA62" s="31"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="23"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="23"/>
+      <c r="O62" s="21"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="22"/>
+      <c r="S62" s="22"/>
+      <c r="T62" s="23"/>
+      <c r="V62" s="21"/>
+      <c r="W62" s="22"/>
+      <c r="X62" s="22"/>
+      <c r="Y62" s="22"/>
+      <c r="Z62" s="22"/>
+      <c r="AA62" s="23"/>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="31"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="30"/>
-      <c r="M63" s="31"/>
-      <c r="O63" s="29"/>
-      <c r="P63" s="30"/>
-      <c r="Q63" s="30"/>
-      <c r="R63" s="30"/>
-      <c r="S63" s="30"/>
-      <c r="T63" s="31"/>
-      <c r="V63" s="29"/>
-      <c r="W63" s="30"/>
-      <c r="X63" s="30"/>
-      <c r="Y63" s="30"/>
-      <c r="Z63" s="30"/>
-      <c r="AA63" s="31"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="23"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="23"/>
+      <c r="O63" s="21"/>
+      <c r="P63" s="22"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="22"/>
+      <c r="S63" s="22"/>
+      <c r="T63" s="23"/>
+      <c r="V63" s="21"/>
+      <c r="W63" s="22"/>
+      <c r="X63" s="22"/>
+      <c r="Y63" s="22"/>
+      <c r="Z63" s="22"/>
+      <c r="AA63" s="23"/>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="31"/>
-      <c r="H64" s="29"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="31"/>
-      <c r="O64" s="29"/>
-      <c r="P64" s="30"/>
-      <c r="Q64" s="30"/>
-      <c r="R64" s="30"/>
-      <c r="S64" s="30"/>
-      <c r="T64" s="31"/>
-      <c r="V64" s="29"/>
-      <c r="W64" s="30"/>
-      <c r="X64" s="30"/>
-      <c r="Y64" s="30"/>
-      <c r="Z64" s="30"/>
-      <c r="AA64" s="31"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="23"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="23"/>
+      <c r="O64" s="21"/>
+      <c r="P64" s="22"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="22"/>
+      <c r="S64" s="22"/>
+      <c r="T64" s="23"/>
+      <c r="V64" s="21"/>
+      <c r="W64" s="22"/>
+      <c r="X64" s="22"/>
+      <c r="Y64" s="22"/>
+      <c r="Z64" s="22"/>
+      <c r="AA64" s="23"/>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="34"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="33"/>
-      <c r="L65" s="33"/>
-      <c r="M65" s="34"/>
-      <c r="O65" s="32"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="33"/>
-      <c r="R65" s="33"/>
-      <c r="S65" s="33"/>
-      <c r="T65" s="34"/>
-      <c r="V65" s="32"/>
-      <c r="W65" s="33"/>
-      <c r="X65" s="33"/>
-      <c r="Y65" s="33"/>
-      <c r="Z65" s="33"/>
-      <c r="AA65" s="34"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="26"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="26"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="25"/>
+      <c r="Q65" s="25"/>
+      <c r="R65" s="25"/>
+      <c r="S65" s="25"/>
+      <c r="T65" s="26"/>
+      <c r="V65" s="24"/>
+      <c r="W65" s="25"/>
+      <c r="X65" s="25"/>
+      <c r="Y65" s="25"/>
+      <c r="Z65" s="25"/>
+      <c r="AA65" s="26"/>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="20"/>
-      <c r="H66" s="18" t="s">
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="29"/>
+      <c r="H66" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
-      <c r="M66" s="20"/>
-      <c r="O66" s="18" t="s">
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="29"/>
+      <c r="O66" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="P66" s="19"/>
-      <c r="Q66" s="19"/>
-      <c r="R66" s="19"/>
-      <c r="S66" s="19"/>
-      <c r="T66" s="20"/>
-      <c r="V66" s="18" t="s">
+      <c r="P66" s="28"/>
+      <c r="Q66" s="28"/>
+      <c r="R66" s="28"/>
+      <c r="S66" s="28"/>
+      <c r="T66" s="29"/>
+      <c r="V66" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="W66" s="19"/>
-      <c r="X66" s="19"/>
-      <c r="Y66" s="19"/>
-      <c r="Z66" s="19"/>
-      <c r="AA66" s="20"/>
+      <c r="W66" s="28"/>
+      <c r="X66" s="28"/>
+      <c r="Y66" s="28"/>
+      <c r="Z66" s="28"/>
+      <c r="AA66" s="29"/>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A67" s="21"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="23"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="23"/>
-      <c r="O67" s="21"/>
-      <c r="P67" s="22"/>
-      <c r="Q67" s="22"/>
-      <c r="R67" s="22"/>
-      <c r="S67" s="22"/>
-      <c r="T67" s="23"/>
-      <c r="V67" s="21"/>
-      <c r="W67" s="22"/>
-      <c r="X67" s="22"/>
-      <c r="Y67" s="22"/>
-      <c r="Z67" s="22"/>
-      <c r="AA67" s="23"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="32"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31"/>
+      <c r="K67" s="31"/>
+      <c r="L67" s="31"/>
+      <c r="M67" s="32"/>
+      <c r="O67" s="30"/>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="31"/>
+      <c r="S67" s="31"/>
+      <c r="T67" s="32"/>
+      <c r="V67" s="30"/>
+      <c r="W67" s="31"/>
+      <c r="X67" s="31"/>
+      <c r="Y67" s="31"/>
+      <c r="Z67" s="31"/>
+      <c r="AA67" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A7:F14"/>
-    <mergeCell ref="A15:F16"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H7:M14"/>
-    <mergeCell ref="H15:M16"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O7:T14"/>
-    <mergeCell ref="O15:T16"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V7:AA14"/>
-    <mergeCell ref="V15:AA16"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="A24:F31"/>
-    <mergeCell ref="H24:M31"/>
-    <mergeCell ref="O24:T31"/>
-    <mergeCell ref="V24:AA31"/>
-    <mergeCell ref="A32:F33"/>
-    <mergeCell ref="H32:M33"/>
-    <mergeCell ref="O32:T33"/>
-    <mergeCell ref="V32:AA33"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="V38:W38"/>
-    <mergeCell ref="A41:F48"/>
-    <mergeCell ref="H41:M48"/>
-    <mergeCell ref="O41:T48"/>
-    <mergeCell ref="V41:AA48"/>
-    <mergeCell ref="A49:F50"/>
-    <mergeCell ref="H49:M50"/>
-    <mergeCell ref="O49:T50"/>
-    <mergeCell ref="V49:AA50"/>
     <mergeCell ref="A66:F67"/>
     <mergeCell ref="H66:M67"/>
     <mergeCell ref="O66:T67"/>
@@ -3912,6 +3876,42 @@
     <mergeCell ref="H58:M65"/>
     <mergeCell ref="O58:T65"/>
     <mergeCell ref="V58:AA65"/>
+    <mergeCell ref="A41:F48"/>
+    <mergeCell ref="H41:M48"/>
+    <mergeCell ref="O41:T48"/>
+    <mergeCell ref="V41:AA48"/>
+    <mergeCell ref="A49:F50"/>
+    <mergeCell ref="H49:M50"/>
+    <mergeCell ref="O49:T50"/>
+    <mergeCell ref="V49:AA50"/>
+    <mergeCell ref="A32:F33"/>
+    <mergeCell ref="H32:M33"/>
+    <mergeCell ref="O32:T33"/>
+    <mergeCell ref="V32:AA33"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="A24:F31"/>
+    <mergeCell ref="H24:M31"/>
+    <mergeCell ref="O24:T31"/>
+    <mergeCell ref="V24:AA31"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O7:T14"/>
+    <mergeCell ref="O15:T16"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V7:AA14"/>
+    <mergeCell ref="V15:AA16"/>
+    <mergeCell ref="A7:F14"/>
+    <mergeCell ref="A15:F16"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H7:M14"/>
+    <mergeCell ref="H15:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>